<commit_message>
added second iteration of assignment 7 (with one dilated kernel)
</commit_message>
<xml_diff>
--- a/Phase-1/Session-7/receptive fields.xlsx
+++ b/Phase-1/Session-7/receptive fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\shyam\Projects\EVA5\personal\Phase-1\Session-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3371457-53B1-465F-AAC0-3A8754341D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A0C71-5CF6-41D9-8D6F-BC6194840EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -259,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -278,6 +278,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="8">
         <v>3</v>
@@ -1373,7 +1374,7 @@
       </c>
       <c r="K8" s="8">
         <f>FLOOR(((J8+2*D8-F8*(C8-1)-1)/E8)+1, 1)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L8" s="8">
         <f>L7+(C8-1)*I8</f>
@@ -1412,11 +1413,11 @@
       </c>
       <c r="J9" s="8">
         <f t="shared" ref="J9:J23" si="1">K8</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" ref="K9:K23" si="2">FLOOR(((J9+2*D9-F9*(C9-1)-1)/E9)+1, 1)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" ref="L9:L23" si="3">L8+(C9-1)*I9</f>
@@ -1456,11 +1457,11 @@
       </c>
       <c r="J10" s="6">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="3"/>
@@ -1497,11 +1498,11 @@
       </c>
       <c r="J11" s="8">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K11" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="8">
         <f t="shared" si="3"/>
@@ -1541,11 +1542,11 @@
       </c>
       <c r="J12" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="3"/>
@@ -1587,11 +1588,11 @@
       </c>
       <c r="J13" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13" s="8">
         <f t="shared" si="3"/>
@@ -1630,11 +1631,11 @@
       </c>
       <c r="J14" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L14" s="8">
         <f t="shared" si="3"/>
@@ -1674,11 +1675,11 @@
       </c>
       <c r="J15" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="3"/>
@@ -1716,7 +1717,7 @@
       </c>
       <c r="J16" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" s="8">
         <f t="shared" si="2"/>
@@ -2051,8 +2052,8 @@
       <c r="L25" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="11">
-        <v>0.83279999999999998</v>
+      <c r="M25" s="14">
+        <v>0.80230000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added readme, updated rf
</commit_message>
<xml_diff>
--- a/Phase-1/Session-7/receptive fields.xlsx
+++ b/Phase-1/Session-7/receptive fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\shyam\Projects\EVA5\personal\Phase-1\Session-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE290481-9F89-4DF3-A095-94C48814C23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B1E860-A7DF-44B5-A2B6-D4BF133278A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="29">
   <si>
     <t>Formulas</t>
   </si>
@@ -169,7 +169,13 @@
     <t>Depthwise Conv2d</t>
   </si>
   <si>
-    <t>Max accuracy</t>
+    <t>Depthwise branch</t>
+  </si>
+  <si>
+    <t>Dilation branch</t>
+  </si>
+  <si>
+    <t>Dilation Conv2d</t>
   </si>
 </sst>
 </file>
@@ -1247,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,568 +1267,1003 @@
     <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M7" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="K7">
+      <c r="O7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <v>32</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>32</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>2</v>
-      </c>
-      <c r="G8" s="8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="8">
-        <v>32</v>
-      </c>
-      <c r="I8" s="8">
-        <f>M7</f>
-        <v>1</v>
-      </c>
-      <c r="J8" s="8">
-        <f>K7</f>
-        <v>32</v>
-      </c>
-      <c r="K8" s="8">
-        <f>FLOOR(((J8+2*D8-F8*(C8-1)-1)/E8)+1, 1)</f>
-        <v>30</v>
-      </c>
-      <c r="L8" s="8">
-        <f>L7+(C8-1)*I8</f>
-        <v>3</v>
-      </c>
-      <c r="M8" s="8">
-        <f>I8*E8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
         <v>32</v>
       </c>
-      <c r="H9">
+      <c r="I9" s="8">
+        <f>M8</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <f>K8</f>
+        <v>32</v>
+      </c>
+      <c r="K9" s="8">
+        <f>FLOOR(((J9+2*D9-F9*(C9-1)-1)/E9)+1, 1)</f>
+        <v>32</v>
+      </c>
+      <c r="L9" s="8">
+        <f>L8+(C9-1)*I9</f>
+        <v>3</v>
+      </c>
+      <c r="M9" s="8">
+        <f>I9*E9</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>3</v>
+      </c>
+      <c r="R9" s="8">
+        <v>2</v>
+      </c>
+      <c r="S9" s="8">
+        <v>1</v>
+      </c>
+      <c r="T9" s="8">
+        <v>2</v>
+      </c>
+      <c r="U9" s="8">
+        <v>3</v>
+      </c>
+      <c r="V9" s="8">
+        <v>32</v>
+      </c>
+      <c r="W9" s="8">
+        <f>AA8</f>
+        <v>1</v>
+      </c>
+      <c r="X9" s="8">
+        <f>Y8</f>
+        <v>32</v>
+      </c>
+      <c r="Y9" s="8">
+        <f>FLOOR(((X9+2*R9-T9*(Q9-1)-1)/S9)+1, 1)</f>
+        <v>32</v>
+      </c>
+      <c r="Z9" s="8">
+        <f>Z8+(Q9-1)*W9</f>
+        <v>3</v>
+      </c>
+      <c r="AA9" s="8">
+        <f>W9*S9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+      <c r="H10">
         <v>64</v>
       </c>
-      <c r="I9" s="8">
-        <f t="shared" ref="I9:I23" si="0">M8</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="shared" ref="J9:J23" si="1">K8</f>
-        <v>30</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" ref="K9:K23" si="2">FLOOR(((J9+2*D9-F9*(C9-1)-1)/E9)+1, 1)</f>
-        <v>30</v>
-      </c>
-      <c r="L9" s="8">
-        <f t="shared" ref="L9:L23" si="3">L8+(C9-1)*I9</f>
+      <c r="I10" s="8">
+        <f t="shared" ref="I10:I24" si="0">M9</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" ref="J10:J24" si="1">K9</f>
+        <v>32</v>
+      </c>
+      <c r="K10" s="8">
+        <f t="shared" ref="K10:K24" si="2">FLOOR(((J10+2*D10-F10*(C10-1)-1)/E10)+1, 1)</f>
+        <v>32</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" ref="L10:L24" si="3">L9+(C10-1)*I10</f>
         <v>5</v>
       </c>
-      <c r="M9" s="8">
-        <f t="shared" ref="M9:M23" si="4">I9*E9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
+      <c r="M10" s="8">
+        <f t="shared" ref="M10:M24" si="4">I10*E10</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10" s="8">
+        <v>2</v>
+      </c>
+      <c r="S10" s="8">
+        <v>1</v>
+      </c>
+      <c r="T10" s="8">
+        <v>2</v>
+      </c>
+      <c r="U10">
+        <v>32</v>
+      </c>
+      <c r="V10">
+        <v>64</v>
+      </c>
+      <c r="W10" s="8">
+        <f t="shared" ref="W10:W24" si="5">AA9</f>
+        <v>1</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" ref="X10:X24" si="6">Y9</f>
+        <v>32</v>
+      </c>
+      <c r="Y10" s="8">
+        <f t="shared" ref="Y10:Y24" si="7">FLOOR(((X10+2*R10-T10*(Q10-1)-1)/S10)+1, 1)</f>
+        <v>32</v>
+      </c>
+      <c r="Z10" s="8">
+        <f t="shared" ref="Z10:Z18" si="8">Z9+(Q10-1)*W10</f>
+        <v>5</v>
+      </c>
+      <c r="AA10" s="8">
+        <f t="shared" ref="AA10:AA24" si="9">W10*S10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>3</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
         <v>64</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H11" s="6">
         <v>128</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I11" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J11" s="6">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="K10" s="6">
+        <v>32</v>
+      </c>
+      <c r="K11" s="6">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="L10" s="6">
+        <v>32</v>
+      </c>
+      <c r="L11" s="6">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M11" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>3</v>
+      </c>
+      <c r="R11" s="6">
+        <v>2</v>
+      </c>
+      <c r="S11" s="6">
+        <v>1</v>
+      </c>
+      <c r="T11" s="6">
+        <v>2</v>
+      </c>
+      <c r="U11" s="6">
+        <v>64</v>
+      </c>
+      <c r="V11" s="6">
+        <v>128</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="X11" s="6">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="Z11" s="6">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AA11" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C12" s="7">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7">
         <v>0</v>
       </c>
-      <c r="E11" s="7">
-        <v>2</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="I11" s="8">
+      <c r="E12" s="7">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="I12" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J12" s="8">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="K11" s="8">
+        <v>32</v>
+      </c>
+      <c r="K12" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="L11" s="8">
+        <v>16</v>
+      </c>
+      <c r="L12" s="8">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M12" s="8">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
+      <c r="O12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>2</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0</v>
+      </c>
+      <c r="S12" s="7">
+        <v>2</v>
+      </c>
+      <c r="T12" s="7">
+        <v>1</v>
+      </c>
+      <c r="U12" s="7"/>
+      <c r="W12" s="8">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="Y12" s="8">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="Z12" s="8">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AA12" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
         <v>0</v>
       </c>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
         <v>128</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H13" s="9">
         <v>32</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I13" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J13" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="K12" s="6">
+        <v>16</v>
+      </c>
+      <c r="K13" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="L12" s="6">
+        <v>16</v>
+      </c>
+      <c r="L13" s="6">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M13" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="O13" s="6"/>
+      <c r="P13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>1</v>
+      </c>
+      <c r="R13" s="9">
+        <v>0</v>
+      </c>
+      <c r="S13" s="9">
+        <v>1</v>
+      </c>
+      <c r="T13" s="9">
+        <v>1</v>
+      </c>
+      <c r="U13" s="9">
+        <v>128</v>
+      </c>
+      <c r="V13" s="9">
+        <v>32</v>
+      </c>
+      <c r="W13" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X13" s="6">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="Y13" s="6">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="Z13" s="6">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AA13" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>32</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>64</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I14" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J14" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="K13" s="8">
+        <v>16</v>
+      </c>
+      <c r="K14" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="L13" s="8">
+        <v>16</v>
+      </c>
+      <c r="L14" s="8">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M14" s="8">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+      <c r="U14">
+        <v>32</v>
+      </c>
+      <c r="V14">
+        <v>64</v>
+      </c>
+      <c r="W14" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X14" s="8">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Y14" s="8">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="Z14" s="8">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="AA14" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
         <v>64</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>128</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I15" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J15" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="K14" s="8">
+        <v>16</v>
+      </c>
+      <c r="K15" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="L14" s="8">
+        <v>16</v>
+      </c>
+      <c r="L15" s="8">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M15" s="8">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+      <c r="P15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>64</v>
+      </c>
+      <c r="V15">
+        <v>128</v>
+      </c>
+      <c r="W15" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X15" s="8">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Y15" s="8">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="Z15" s="8">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="AA15" s="8">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C16" s="6">
         <v>3</v>
       </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
         <v>128</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H16" s="6">
         <v>256</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I16" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J16" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="K15" s="6">
+        <v>16</v>
+      </c>
+      <c r="K16" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="L15" s="6">
+        <v>16</v>
+      </c>
+      <c r="L16" s="6">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M16" s="6">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="6">
+        <v>3</v>
+      </c>
+      <c r="R16" s="6">
+        <v>2</v>
+      </c>
+      <c r="S16" s="6">
+        <v>1</v>
+      </c>
+      <c r="T16" s="6">
+        <v>2</v>
+      </c>
+      <c r="U16" s="6">
+        <v>128</v>
+      </c>
+      <c r="V16" s="6">
+        <v>256</v>
+      </c>
+      <c r="W16" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X16" s="6">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Y16" s="6">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="Z16" s="6">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="AA16" s="6">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="7">
-        <v>2</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
         <v>0</v>
       </c>
-      <c r="E16" s="7">
-        <v>2</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8">
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J17" s="8">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="K16" s="8">
+        <v>16</v>
+      </c>
+      <c r="K17" s="8">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="L16" s="8">
+        <v>8</v>
+      </c>
+      <c r="L17" s="8">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M17" s="8">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="9" t="s">
+      <c r="O17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>2</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0</v>
+      </c>
+      <c r="S17" s="7">
+        <v>2</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="X17" s="8">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Y17" s="8">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z17" s="8">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="AA17" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+      <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="9">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="C18" s="9">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9">
         <v>0</v>
       </c>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9">
         <v>256</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H18" s="9">
         <v>64</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J18" s="6">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="K17" s="6">
+        <v>8</v>
+      </c>
+      <c r="K18" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="L17" s="6">
+        <v>8</v>
+      </c>
+      <c r="L18" s="6">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M18" s="6">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="O18" s="6"/>
+      <c r="P18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>1</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0</v>
+      </c>
+      <c r="S18" s="9">
+        <v>1</v>
+      </c>
+      <c r="T18" s="9">
+        <v>1</v>
+      </c>
+      <c r="U18" s="9">
+        <v>256</v>
+      </c>
+      <c r="V18" s="9">
+        <v>64</v>
+      </c>
+      <c r="W18" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="X18" s="6">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="Y18" s="6">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z18" s="6">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="AA18" s="6">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>64</v>
-      </c>
-      <c r="H18">
-        <v>128</v>
-      </c>
-      <c r="I18" s="8">
-        <f>M17</f>
-        <v>4</v>
-      </c>
-      <c r="J18" s="8">
-        <f>K17</f>
-        <v>7</v>
-      </c>
-      <c r="K18" s="8">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="L18" s="8">
-        <f>L17+(C18-1)*I18</f>
-        <v>30</v>
-      </c>
-      <c r="M18" s="8">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>25</v>
       </c>
@@ -1839,122 +2280,255 @@
         <v>1</v>
       </c>
       <c r="G19">
+        <v>64</v>
+      </c>
+      <c r="H19">
         <v>128</v>
       </c>
-      <c r="H19">
-        <v>256</v>
-      </c>
       <c r="I19" s="8">
-        <f t="shared" si="0"/>
+        <f>M18</f>
         <v>4</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>K18</f>
+        <v>8</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" si="3"/>
-        <v>38</v>
+        <f>L18+(C19-1)*I19</f>
+        <v>30</v>
       </c>
       <c r="M19" s="8">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="O19" t="s">
+        <v>24</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <v>2</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>2</v>
+      </c>
+      <c r="U19">
+        <v>64</v>
+      </c>
+      <c r="V19">
+        <v>128</v>
+      </c>
+      <c r="W19" s="8">
+        <f>AA18</f>
+        <v>4</v>
+      </c>
+      <c r="X19" s="8">
+        <f>Y18</f>
+        <v>8</v>
+      </c>
+      <c r="Y19" s="8">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z19" s="8">
+        <f>Z18+(Q19-1)*W19</f>
+        <v>30</v>
+      </c>
+      <c r="AA19" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" s="6">
-        <v>1</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>128</v>
+      </c>
+      <c r="H20">
         <v>256</v>
       </c>
-      <c r="H20" s="6">
-        <v>256</v>
-      </c>
-      <c r="I20" s="6">
+      <c r="I20" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="8">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="K20" s="6">
+        <v>8</v>
+      </c>
+      <c r="K20" s="8">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="L20" s="6">
+        <v>8</v>
+      </c>
+      <c r="L20" s="8">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="M20" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>2</v>
+      </c>
+      <c r="U20">
+        <v>128</v>
+      </c>
+      <c r="V20">
+        <v>256</v>
+      </c>
+      <c r="W20" s="8">
+        <f t="shared" ref="W20:W24" si="10">AA19</f>
+        <v>4</v>
+      </c>
+      <c r="X20" s="8">
+        <f t="shared" ref="X20:X24" si="11">Y19</f>
+        <v>8</v>
+      </c>
+      <c r="Y20" s="8">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z20" s="8">
+        <f t="shared" ref="Z20:Z24" si="12">Z19+(Q20-1)*W20</f>
+        <v>38</v>
+      </c>
+      <c r="AA20" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6">
+        <v>3</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>256</v>
+      </c>
+      <c r="H21" s="6">
+        <v>256</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L21" s="6">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M21" s="6">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="O21" s="6"/>
+      <c r="P21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>3</v>
+      </c>
+      <c r="R21" s="6">
+        <v>2</v>
+      </c>
+      <c r="S21" s="6">
+        <v>1</v>
+      </c>
+      <c r="T21" s="6">
+        <v>2</v>
+      </c>
+      <c r="U21" s="6">
+        <v>256</v>
+      </c>
+      <c r="V21" s="6">
+        <v>256</v>
+      </c>
+      <c r="W21" s="6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="X21" s="6">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="Y21" s="6">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z21" s="6">
+        <f t="shared" si="12"/>
+        <v>46</v>
+      </c>
+      <c r="AA21" s="6">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="7">
-        <v>7</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="I21" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J21" s="8">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="K21" s="8">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L21" s="8">
-        <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="M21" s="8">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="C22" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D22" s="7">
         <v>0</v>
@@ -1964,12 +2538,6 @@
       </c>
       <c r="F22" s="7">
         <v>1</v>
-      </c>
-      <c r="G22" s="7">
-        <v>256</v>
-      </c>
-      <c r="H22" s="7">
-        <v>64</v>
       </c>
       <c r="I22" s="8">
         <f t="shared" si="0"/>
@@ -1977,7 +2545,7 @@
       </c>
       <c r="J22" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="2"/>
@@ -1985,126 +2553,270 @@
       </c>
       <c r="L22" s="8">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M22" s="8">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="9" t="s">
+      <c r="O22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>8</v>
+      </c>
+      <c r="R22" s="7">
+        <v>0</v>
+      </c>
+      <c r="S22" s="7">
+        <v>1</v>
+      </c>
+      <c r="T22" s="7">
+        <v>1</v>
+      </c>
+      <c r="W22" s="8">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="X22" s="8">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="Y22" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Z22" s="8">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="AA22" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
         <v>0</v>
       </c>
-      <c r="E23" s="9">
-        <v>1</v>
-      </c>
-      <c r="F23" s="9">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6">
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>256</v>
+      </c>
+      <c r="H23" s="7">
         <v>64</v>
       </c>
-      <c r="H23" s="6">
-        <v>10</v>
-      </c>
-      <c r="I23" s="6">
+      <c r="I23" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="8">
         <f t="shared" si="3"/>
-        <v>70</v>
-      </c>
-      <c r="M23" s="6">
+        <v>74</v>
+      </c>
+      <c r="M23" s="8">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L25" t="s">
-        <v>26</v>
-      </c>
-      <c r="M25" s="14">
-        <v>0.80230000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M26" s="11"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
+        <v>0</v>
+      </c>
+      <c r="S23" s="7">
+        <v>1</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7">
+        <v>256</v>
+      </c>
+      <c r="V23" s="7">
+        <v>64</v>
+      </c>
+      <c r="W23" s="8">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="X23" s="8">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Y23" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Z23" s="8">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="AA23" s="8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
+      <c r="B24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>64</v>
+      </c>
+      <c r="H24" s="6">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="M24" s="6">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="O24" s="6"/>
+      <c r="P24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>1</v>
+      </c>
+      <c r="R24" s="9">
+        <v>0</v>
+      </c>
+      <c r="S24" s="9">
+        <v>1</v>
+      </c>
+      <c r="T24" s="9">
+        <v>1</v>
+      </c>
+      <c r="U24" s="6">
+        <v>64</v>
+      </c>
+      <c r="V24" s="6">
+        <v>10</v>
+      </c>
+      <c r="W24" s="6">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="X24" s="6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Y24" s="6">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Z24" s="6">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="AA24" s="6">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="M27" s="11"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2119,7 +2831,7 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2136,12 +2848,12 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2151,12 +2863,12 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -2181,13 +2893,13 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -2196,13 +2908,13 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2226,13 +2938,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -2241,13 +2953,13 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
@@ -2271,13 +2983,13 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
@@ -2286,13 +2998,13 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -2316,13 +3028,13 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -2351,8 +3063,8 @@
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -2377,10 +3089,10 @@
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
@@ -2391,7 +3103,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
@@ -2404,6 +3116,21 @@
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
     </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>